<commit_message>
Latex table imports added
</commit_message>
<xml_diff>
--- a/latex/tables/adapter_workbook.xlsx
+++ b/latex/tables/adapter_workbook.xlsx
@@ -376,9 +376,6 @@
     <t>Lasso</t>
   </si>
   <si>
-    <t>Elastic Net</t>
-  </si>
-  <si>
     <t>Grace</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>LTLP</t>
+  </si>
+  <si>
+    <t>ENet</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:A13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
         <v>89</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>89</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>89</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
         <v>89</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>89</v>
@@ -1784,7 +1784,7 @@
   <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:A13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1800,19 +1800,19 @@
         <v>91</v>
       </c>
       <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>95</v>
-      </c>
-      <c r="H1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -1878,7 +1878,7 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
         <v>89</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>89</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>89</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
         <v>89</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>89</v>
@@ -2581,7 +2581,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B4" t="str">
         <f>FIXED(cvmse_sum_in!B3)</f>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="str">
         <f>FIXED(cvmse_sum_in!B4)</f>
@@ -2749,7 +2749,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" t="str">
         <f>FIXED(cvmse_sum_in!B5)</f>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" t="str">
         <f>FIXED(cvmse_sum_in!B6)</f>
@@ -2843,7 +2843,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" t="str">
         <f>FIXED(cvmse_sum_in!B7)</f>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" t="str">
         <f>FIXED(cvmse_sum_in!B8)</f>
@@ -2937,7 +2937,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" t="str">
         <f>FIXED(cvmse_sum_in!B9)</f>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" t="str">
         <f>FIXED(cvmse_sum_in!B10)</f>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" t="str">
         <f>FIXED(cvmse_sum_in!B11)</f>
@@ -3086,7 +3086,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3493,7 +3493,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B4" t="str">
         <f>FIXED(orctun_sum_in!B3)</f>
@@ -3614,7 +3614,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="str">
         <f>FIXED(orctun_sum_in!B4)</f>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" t="str">
         <f>FIXED(orctun_sum_in!B5)</f>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="str">
         <f>FIXED(orctun_sum_in!B6)</f>
@@ -3755,7 +3755,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" t="str">
         <f>FIXED(orctun_sum_in!B7)</f>
@@ -4077,7 +4077,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4094,31 +4094,31 @@
         <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" t="s">
         <v>95</v>
-      </c>
-      <c r="H1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -4218,7 +4218,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B3, 5))</f>
@@ -4313,7 +4313,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B4, 5))</f>
@@ -4408,7 +4408,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B5, 5))</f>
@@ -4503,7 +4503,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B6, 5))</f>
@@ -4598,7 +4598,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B7, 5))</f>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B8, 5))</f>
@@ -4788,7 +4788,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B9, 5))</f>
@@ -4883,7 +4883,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B10, 5))</f>
@@ -4978,7 +4978,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B11, 5))</f>
@@ -5483,7 +5483,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5496,19 +5496,19 @@
         <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>95</v>
-      </c>
-      <c r="G1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5576,7 +5576,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B3, 5))</f>
@@ -5639,7 +5639,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B4, 5))</f>
@@ -5702,7 +5702,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B5, 5))</f>
@@ -5765,7 +5765,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B6, 5))</f>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B7, 5))</f>

</xml_diff>

<commit_message>
Mapping tables and figures prepared for LaTeX
</commit_message>
<xml_diff>
--- a/latex/tables/adapter_workbook.xlsx
+++ b/latex/tables/adapter_workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28860" windowHeight="6375" activeTab="8"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28860" windowHeight="6375" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="met_comp" sheetId="11" r:id="rId1"/>
@@ -17,10 +17,18 @@
     <sheet name="cvmse_sim_in" sheetId="5" r:id="rId8"/>
     <sheet name="orctun_sim_out" sheetId="7" r:id="rId9"/>
     <sheet name="orctun_sim_in" sheetId="6" r:id="rId10"/>
+    <sheet name="map_errors_out" sheetId="15" r:id="rId11"/>
+    <sheet name="map_errors_in" sheetId="12" r:id="rId12"/>
+    <sheet name="map_sum_out" sheetId="14" r:id="rId13"/>
+    <sheet name="map_sum_in" sheetId="13" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="orctun_results_coef_correlation_p550_summary" localSheetId="5">orctun_sum_in!$A$1:$K$7</definedName>
-    <definedName name="orctun_similarities" localSheetId="9">orctun_sim_in!$A$1:$G$7</definedName>
+    <definedName name="mapping_errors" localSheetId="10">map_errors_out!$A$1:$D$11</definedName>
+    <definedName name="mapping_errors_1" localSheetId="11">map_errors_in!$A$1:$D$11</definedName>
+    <definedName name="mapping_summary" localSheetId="12">map_sum_out!$A$1:$F$11</definedName>
+    <definedName name="mapping_summary_1" localSheetId="13">map_sum_in!$A$1:$F$11</definedName>
+    <definedName name="orctun_results_coef_correlation_p550_summary" localSheetId="5">orctun_sum_in!$A$1:$K$6</definedName>
+    <definedName name="orctun_similarities" localSheetId="9">orctun_sim_in!$A$1:$F$6</definedName>
     <definedName name="p550_summary" localSheetId="3">cvmse_sum_in!$A$1:$K$11</definedName>
     <definedName name="similarities" localSheetId="7">cvmse_sim_in!$A$1:$K$11</definedName>
   </definedNames>
@@ -30,7 +38,51 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="orctun_results_coef_correlation_p550_summary" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="1" name="mapping_errors" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="866" sourceFile="C:\Users\sivak_000\Documents\GitHub\dissertation\python\results\mapping_errors.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="mapping_errors1" type="6" refreshedVersion="3" deleted="1" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="866" sourceFile="C:\Users\sivak_000\Documents\GitHub\dissertation\latex\tables\mapping_errors.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="mapping_summary" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="866" sourceFile="C:\Users\sivak_000\Documents\GitHub\dissertation\python\results\mapping_summary.csv" comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="mapping_summary1" type="6" refreshedVersion="3" deleted="1" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="866" sourceFile="C:\Users\sivak_000\Documents\GitHub\dissertation\latex\tables\mapping_summary.csv" comma="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="orctun_results_coef_correlation_p550_summary" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="866" sourceFile="C:\Users\sivak_000\Documents\GitHub\dissertation\python\results\orctun_results_coef_correlation_p550_summary.csv" comma="1">
       <textFields count="11">
         <textField/>
@@ -47,7 +99,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="orctun_similarities" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="6" name="orctun_similarities" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="866" sourceFile="C:\Users\sivak_000\Documents\GitHub\dissertation\python\results\orctun_similarities.csv" comma="1">
       <textFields count="7">
         <textField/>
@@ -60,7 +112,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="p550_summary" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="7" name="p550_summary" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="866" sourceFile="C:\Users\sivak_000\Documents\GitHub\dissertation\python\results\p550_summary.csv" comma="1">
       <textFields count="11">
         <textField/>
@@ -77,7 +129,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="similarities" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="8" name="similarities" type="6" refreshedVersion="3" background="1" refreshOnLoad="1" saveData="1">
     <textPr prompt="0" codePage="866" sourceFile="C:\Users\sivak_000\Documents\GitHub\dissertation\python\results\similarities.csv" comma="1">
       <textFields count="11">
         <textField/>
@@ -98,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="108">
   <si>
     <t>lasso</t>
   </si>
@@ -280,9 +332,6 @@
     <t>0.855 (0.055)</t>
   </si>
   <si>
-    <t>0.930 (0.026)</t>
-  </si>
-  <si>
     <t>0.949 (0.069)</t>
   </si>
   <si>
@@ -292,27 +341,15 @@
     <t>0.930 (0.024)</t>
   </si>
   <si>
-    <t>0.923 (0.022)</t>
-  </si>
-  <si>
     <t>0.892 (0.058)</t>
   </si>
   <si>
     <t>0.919 (0.033)</t>
   </si>
   <si>
-    <t>0.863 (0.080)</t>
-  </si>
-  <si>
     <t>0.978 (0.010)</t>
   </si>
   <si>
-    <t>0.850 (0.045)</t>
-  </si>
-  <si>
-    <t>0.855 (0.037)</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
@@ -401,6 +438,42 @@
   </si>
   <si>
     <t>ENet</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Prom</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Unresolved</t>
+  </si>
+  <si>
+    <t>Influencing</t>
+  </si>
+  <si>
+    <t>Non-influencing</t>
+  </si>
+  <si>
+    <t>Enet</t>
+  </si>
+  <si>
+    <t>Cell body</t>
+  </si>
+  <si>
+    <t>Promoter</t>
+  </si>
+  <si>
+    <t>Elastic Net</t>
   </si>
 </sst>
 </file>
@@ -893,10 +966,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -948,19 +1022,35 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="p550_summary" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="p550_summary" refreshOnLoad="1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="orctun_results_coef_correlation_p550_summary" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="orctun_results_coef_correlation_p550_summary" refreshOnLoad="1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="similarities" refreshOnLoad="1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="similarities" refreshOnLoad="1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="orctun_similarities" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="orctun_similarities" refreshOnLoad="1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mapping_errors" refreshOnLoad="1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mapping_errors_1" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mapping_summary" refreshOnLoad="1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mapping_summary_1" refreshOnLoad="1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1258,33 +1348,33 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C2" t="str">
         <f>cvmse_sum_out!B2</f>
@@ -1309,7 +1399,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C3" t="str">
         <f>orctun_sum_out!B2</f>
@@ -1334,10 +1424,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4" t="str">
         <f>cvmse_sum_out!B4</f>
@@ -1362,7 +1452,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" t="str">
         <f>orctun_sum_out!B4</f>
@@ -1387,10 +1477,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C6" t="str">
         <f>cvmse_sum_out!B6</f>
@@ -1415,7 +1505,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C7" t="str">
         <f>orctun_sum_out!B6</f>
@@ -1440,10 +1530,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C8" t="str">
         <f>cvmse_sum_out!B10</f>
@@ -1468,7 +1558,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C9" t="str">
         <f>orctun_sum_out!B8</f>
@@ -1493,10 +1583,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C10" t="str">
         <f>cvmse_sum_out!B12</f>
@@ -1521,35 +1611,35 @@
     </row>
     <row r="11" spans="1:7">
       <c r="B11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" t="str">
+        <v>85</v>
+      </c>
+      <c r="C11" t="e">
         <f>orctun_sum_out!B10</f>
-        <v>18.04</v>
-      </c>
-      <c r="D11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="D11" t="e">
         <f>orctun_sum_out!C10</f>
-        <v>0.74</v>
-      </c>
-      <c r="E11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="E11" t="e">
         <f>orctun_sum_out!D10</f>
-        <v>0.99</v>
-      </c>
-      <c r="F11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="F11" t="e">
         <f>orctun_sum_out!E10</f>
-        <v>0.81</v>
-      </c>
-      <c r="G11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="G11" t="e">
         <f>orctun_sum_out!F10</f>
-        <v>0.61</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C12" t="str">
         <f>cvmse_sum_out!B20</f>
@@ -1574,27 +1664,27 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C13" t="str">
         <f>orctun_sum_out!B12</f>
-        <v>26.75</v>
+        <v>18.04</v>
       </c>
       <c r="D13" t="str">
         <f>orctun_sum_out!C12</f>
-        <v>0.69</v>
+        <v>0.74</v>
       </c>
       <c r="E13" t="str">
         <f>orctun_sum_out!D12</f>
-        <v>0.63</v>
+        <v>0.99</v>
       </c>
       <c r="F13" t="str">
         <f>orctun_sum_out!E12</f>
-        <v>0.87</v>
+        <v>0.81</v>
       </c>
       <c r="G13" t="str">
         <f>orctun_sum_out!F12</f>
-        <v>0.59</v>
+        <v>0.61</v>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +1694,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1612,11 +1702,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1632,11 +1722,8 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1655,11 +1742,8 @@
       <c r="F2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1670,19 +1754,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
         <v>61</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>62</v>
       </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1690,22 +1771,19 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1713,22 +1791,19 @@
         <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1736,42 +1811,860 @@
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="3">
+        <f>map_errors_in!C2</f>
+        <v>0.66039587426199997</v>
+      </c>
+      <c r="D2" s="3">
+        <f>map_errors_in!D2</f>
+        <v>0.75375712381000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="3">
+        <f>map_errors_in!C3</f>
+        <v>0.66496958241399995</v>
+      </c>
+      <c r="D3" s="3">
+        <f>map_errors_in!D3</f>
+        <v>0.73970676751999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="3">
+        <f>map_errors_in!C4</f>
+        <v>0.65453684774700005</v>
+      </c>
+      <c r="D4" s="3">
+        <f>map_errors_in!D4</f>
+        <v>0.72775155569100003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="3">
+        <f>map_errors_in!C5</f>
+        <v>0.66811830673999995</v>
+      </c>
+      <c r="D5" s="3">
+        <f>map_errors_in!D5</f>
+        <v>0.74596253970799997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="3">
+        <f>map_errors_in!C6</f>
+        <v>0.68068092973700001</v>
+      </c>
+      <c r="D6" s="3">
+        <f>map_errors_in!D6</f>
+        <v>0.81279036388799997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="3">
+        <f>map_errors_in!C7</f>
+        <v>0.65025996691599997</v>
+      </c>
+      <c r="D7" s="3">
+        <f>map_errors_in!D7</f>
+        <v>0.69938890352600003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="3">
+        <f>map_errors_in!C8</f>
+        <v>0.67349601159899997</v>
+      </c>
+      <c r="D8" s="3">
+        <f>map_errors_in!D8</f>
+        <v>0.74849381868700005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="3">
+        <f>map_errors_in!C9</f>
+        <v>0.65959871546000004</v>
+      </c>
+      <c r="D9" s="3">
+        <f>map_errors_in!D9</f>
+        <v>0.72229100217300002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="3">
+        <f>map_errors_in!C10</f>
+        <v>0.67677408699399999</v>
+      </c>
+      <c r="D10" s="3">
+        <f>map_errors_in!D10</f>
+        <v>0.75244165631000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="3">
+        <f>map_errors_in!C11</f>
+        <v>0.70187944185399997</v>
+      </c>
+      <c r="D11" s="3">
+        <f>map_errors_in!D11</f>
+        <v>0.85630315789400002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
+      <c r="C2">
+        <v>0.66039587426199997</v>
+      </c>
+      <c r="D2">
+        <v>0.75375712381000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.66496958241399995</v>
+      </c>
+      <c r="D3">
+        <v>0.73970676751999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.65453684774700005</v>
+      </c>
+      <c r="D4">
+        <v>0.72775155569100003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.66811830673999995</v>
+      </c>
+      <c r="D5">
+        <v>0.74596253970799997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.68068092973700001</v>
+      </c>
+      <c r="D6">
+        <v>0.81279036388799997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
       <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>0.65025996691599997</v>
+      </c>
+      <c r="D7">
+        <v>0.69938890352600003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.67349601159899997</v>
+      </c>
+      <c r="D8">
+        <v>0.74849381868700005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>0.65959871546000004</v>
+      </c>
+      <c r="D9">
+        <v>0.72229100217300002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0.67677408699399999</v>
+      </c>
+      <c r="D10">
+        <v>0.75244165631000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0.70187944185399997</v>
+      </c>
+      <c r="D11">
+        <v>0.85630315789400002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="A1:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2">
+        <f>map_sum_in!C2</f>
+        <v>471</v>
+      </c>
+      <c r="D2">
+        <f>map_sum_in!D2</f>
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <f>map_sum_in!E2</f>
+        <v>206</v>
+      </c>
+      <c r="F2">
+        <f>map_sum_in!F2</f>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3">
+        <f>map_sum_in!C3</f>
+        <v>473</v>
+      </c>
+      <c r="D3">
+        <f>map_sum_in!D3</f>
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <f>map_sum_in!E3</f>
+        <v>242</v>
+      </c>
+      <c r="F3">
+        <f>map_sum_in!F3</f>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4">
+        <f>map_sum_in!C4</f>
+        <v>474</v>
+      </c>
+      <c r="D4">
+        <f>map_sum_in!D4</f>
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f>map_sum_in!E4</f>
+        <v>234</v>
+      </c>
+      <c r="F4">
+        <f>map_sum_in!F4</f>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5">
+        <f>map_sum_in!C5</f>
+        <v>470</v>
+      </c>
+      <c r="D5">
+        <f>map_sum_in!D5</f>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f>map_sum_in!E5</f>
+        <v>205</v>
+      </c>
+      <c r="F5">
+        <f>map_sum_in!F5</f>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6">
+        <f>map_sum_in!C6</f>
+        <v>479</v>
+      </c>
+      <c r="D6">
+        <f>map_sum_in!D6</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>map_sum_in!E6</f>
+        <v>307</v>
+      </c>
+      <c r="F6">
+        <f>map_sum_in!F6</f>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7">
+        <f>map_sum_in!C7</f>
+        <v>455</v>
+      </c>
+      <c r="D7">
+        <f>map_sum_in!D7</f>
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <f>map_sum_in!E7</f>
+        <v>155</v>
+      </c>
+      <c r="F7">
+        <f>map_sum_in!F7</f>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8">
+        <f>map_sum_in!C8</f>
+        <v>458</v>
+      </c>
+      <c r="D8">
+        <f>map_sum_in!D8</f>
         <v>10</v>
+      </c>
+      <c r="E8">
+        <f>map_sum_in!E8</f>
+        <v>166</v>
+      </c>
+      <c r="F8">
+        <f>map_sum_in!F8</f>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9">
+        <f>map_sum_in!C9</f>
+        <v>461</v>
+      </c>
+      <c r="D9">
+        <f>map_sum_in!D9</f>
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f>map_sum_in!E9</f>
+        <v>175</v>
+      </c>
+      <c r="F9">
+        <f>map_sum_in!F9</f>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10">
+        <f>map_sum_in!C10</f>
+        <v>453</v>
+      </c>
+      <c r="D10">
+        <f>map_sum_in!D10</f>
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <f>map_sum_in!E10</f>
+        <v>151</v>
+      </c>
+      <c r="F10">
+        <f>map_sum_in!F10</f>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11">
+        <f>map_sum_in!C11</f>
+        <v>468</v>
+      </c>
+      <c r="D11">
+        <f>map_sum_in!D11</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>map_sum_in!E11</f>
+        <v>468</v>
+      </c>
+      <c r="F11">
+        <f>map_sum_in!F11</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J41" sqref="J41:J45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2">
+        <v>471</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>206</v>
+      </c>
+      <c r="F2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3">
+        <v>473</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>242</v>
+      </c>
+      <c r="F3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4">
+        <v>474</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>234</v>
+      </c>
+      <c r="F4">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5">
+        <v>470</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>205</v>
+      </c>
+      <c r="F5">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6">
+        <v>479</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>307</v>
+      </c>
+      <c r="F6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7">
+        <v>455</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>155</v>
+      </c>
+      <c r="F7">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8">
+        <v>458</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>166</v>
+      </c>
+      <c r="F8">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9">
+        <v>461</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>175</v>
+      </c>
+      <c r="F9">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10">
+        <v>453</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>151</v>
+      </c>
+      <c r="F10">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11">
+        <v>468</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>468</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1791,36 +2684,36 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C2" t="str">
         <f>cvmse_sim_out!B2</f>
@@ -1849,7 +2742,7 @@
     </row>
     <row r="3" spans="1:26">
       <c r="B3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C3" t="str">
         <f>orctun_sim_out!B2</f>
@@ -1871,17 +2764,17 @@
         <f>orctun_sim_out!F2</f>
         <v>0.86</v>
       </c>
-      <c r="H3" t="str">
+      <c r="H3" t="e">
         <f>orctun_sim_out!G2</f>
-        <v>0.93</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C4" t="str">
         <f>cvmse_sim_out!B4</f>
@@ -1910,7 +2803,7 @@
     </row>
     <row r="5" spans="1:26">
       <c r="B5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" t="str">
         <f>orctun_sim_out!B4</f>
@@ -1932,17 +2825,17 @@
         <f>orctun_sim_out!F4</f>
         <v>0.93</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H5" t="e">
         <f>orctun_sim_out!G4</f>
-        <v>0.92</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C6" t="str">
         <f>cvmse_sim_out!B6</f>
@@ -1971,7 +2864,7 @@
     </row>
     <row r="7" spans="1:26">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C7" t="str">
         <f>orctun_sim_out!B6</f>
@@ -1993,17 +2886,17 @@
         <f>orctun_sim_out!F6</f>
         <v>0.92</v>
       </c>
-      <c r="H7" t="str">
+      <c r="H7" t="e">
         <f>orctun_sim_out!G6</f>
-        <v>0.86</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C8" t="str">
         <f>cvmse_sim_out!B10</f>
@@ -2032,7 +2925,7 @@
     </row>
     <row r="9" spans="1:26">
       <c r="B9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C9" t="str">
         <f>orctun_sim_out!B8</f>
@@ -2054,17 +2947,17 @@
         <f>orctun_sim_out!F8</f>
         <v>0.98</v>
       </c>
-      <c r="H9" t="str">
+      <c r="H9" t="e">
         <f>orctun_sim_out!G8</f>
-        <v>0.85</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C10" t="str">
         <f>cvmse_sim_out!B12</f>
@@ -2093,39 +2986,39 @@
     </row>
     <row r="11" spans="1:26">
       <c r="B11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" t="str">
+        <v>85</v>
+      </c>
+      <c r="C11" t="e">
         <f>orctun_sim_out!B10</f>
-        <v>0.86</v>
-      </c>
-      <c r="D11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="D11" t="e">
         <f>orctun_sim_out!C10</f>
-        <v>0.93</v>
-      </c>
-      <c r="E11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="E11" t="e">
         <f>orctun_sim_out!D10</f>
-        <v>0.92</v>
-      </c>
-      <c r="F11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="F11" t="e">
         <f>orctun_sim_out!E10</f>
-        <v>0.98</v>
-      </c>
-      <c r="G11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="G11" t="e">
         <f>orctun_sim_out!F10</f>
-        <v>1.00</v>
-      </c>
-      <c r="H11" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="H11" t="e">
         <f>orctun_sim_out!G10</f>
-        <v>0.86</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C12" t="str">
         <f>cvmse_sim_out!B20</f>
@@ -2154,31 +3047,31 @@
     </row>
     <row r="13" spans="1:26">
       <c r="B13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C13" t="str">
         <f>orctun_sim_out!B12</f>
-        <v>0.93</v>
+        <v>0.86</v>
       </c>
       <c r="D13" t="str">
         <f>orctun_sim_out!C12</f>
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="E13" t="str">
         <f>orctun_sim_out!D12</f>
-        <v>0.86</v>
+        <v>0.92</v>
       </c>
       <c r="F13" t="str">
         <f>orctun_sim_out!E12</f>
-        <v>0.85</v>
+        <v>0.98</v>
       </c>
       <c r="G13" t="str">
         <f>orctun_sim_out!F12</f>
-        <v>0.86</v>
-      </c>
-      <c r="H13" t="str">
+        <v>1.00</v>
+      </c>
+      <c r="H13" t="e">
         <f>orctun_sim_out!G12</f>
-        <v>1.00</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -2588,27 +3481,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" t="s">
-        <v>87</v>
-      </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" t="str">
         <f>FIXED(cvmse_sum_in!B2)</f>
@@ -2655,7 +3548,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B4" t="str">
         <f>FIXED(cvmse_sum_in!B3)</f>
@@ -2702,7 +3595,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B6" t="str">
         <f>FIXED(cvmse_sum_in!B4)</f>
@@ -2749,7 +3642,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B8" t="str">
         <f>FIXED(cvmse_sum_in!B5)</f>
@@ -2796,7 +3689,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B10" t="str">
         <f>FIXED(cvmse_sum_in!B6)</f>
@@ -2843,7 +3736,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B12" t="str">
         <f>FIXED(cvmse_sum_in!B7)</f>
@@ -2890,7 +3783,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B14" t="str">
         <f>FIXED(cvmse_sum_in!B8)</f>
@@ -2937,7 +3830,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B16" t="str">
         <f>FIXED(cvmse_sum_in!B9)</f>
@@ -2984,7 +3877,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B18" t="str">
         <f>FIXED(cvmse_sum_in!B10)</f>
@@ -3031,7 +3924,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B20" t="str">
         <f>FIXED(cvmse_sum_in!B11)</f>
@@ -3100,37 +3993,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -3500,27 +4393,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" t="s">
-        <v>87</v>
-      </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" t="str">
         <f>FIXED(orctun_sum_in!B2)</f>
@@ -3567,7 +4460,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B4" t="str">
         <f>FIXED(orctun_sum_in!B3)</f>
@@ -3614,7 +4507,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B6" t="str">
         <f>FIXED(orctun_sum_in!B4)</f>
@@ -3661,7 +4554,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B8" t="str">
         <f>FIXED(orctun_sum_in!B5)</f>
@@ -3708,95 +4601,95 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" t="str">
+        <v>89</v>
+      </c>
+      <c r="B10" t="e">
+        <f>FIXED(orctun_sum_in!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C10" t="e">
+        <f>FIXED(orctun_sum_in!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D10" t="e">
+        <f>FIXED(orctun_sum_in!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E10" t="e">
+        <f>FIXED(orctun_sum_in!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F10" t="e">
+        <f>FIXED(orctun_sum_in!#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="e">
+        <f>CONCATENATE("(",FIXED(orctun_sum_in!#REF!),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C11" t="e">
+        <f>CONCATENATE("(",FIXED(orctun_sum_in!#REF!),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D11" t="e">
+        <f>CONCATENATE("(",FIXED(orctun_sum_in!#REF!),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E11" t="e">
+        <f>CONCATENATE("(",FIXED(orctun_sum_in!#REF!),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F11" t="e">
+        <f>CONCATENATE("(",FIXED(orctun_sum_in!#REF!),")")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="str">
         <f>FIXED(orctun_sum_in!B6)</f>
         <v>18.04</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C12" t="str">
         <f>FIXED(orctun_sum_in!D6)</f>
         <v>0.74</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D12" t="str">
         <f>FIXED(orctun_sum_in!F6)</f>
         <v>0.99</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E12" t="str">
         <f>FIXED(orctun_sum_in!H6)</f>
         <v>0.81</v>
       </c>
-      <c r="F10" t="str">
+      <c r="F12" t="str">
         <f>FIXED(orctun_sum_in!J6)</f>
         <v>0.61</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="B11" t="str">
+    <row r="13" spans="1:6">
+      <c r="B13" t="str">
         <f>CONCATENATE("(",FIXED(orctun_sum_in!C6),")")</f>
         <v>(11.99)</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C13" t="str">
         <f>CONCATENATE("(",FIXED(orctun_sum_in!E6),")")</f>
         <v>(0.15)</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D13" t="str">
         <f>CONCATENATE("(",FIXED(orctun_sum_in!G6),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E13" t="str">
         <f>CONCATENATE("(",FIXED(orctun_sum_in!I6),")")</f>
         <v>(0.11)</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F13" t="str">
         <f>CONCATENATE("(",FIXED(orctun_sum_in!K6),")")</f>
-        <v>(0.22)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" t="str">
-        <f>FIXED(orctun_sum_in!B7)</f>
-        <v>26.75</v>
-      </c>
-      <c r="C12" t="str">
-        <f>FIXED(orctun_sum_in!D7)</f>
-        <v>0.69</v>
-      </c>
-      <c r="D12" t="str">
-        <f>FIXED(orctun_sum_in!F7)</f>
-        <v>0.63</v>
-      </c>
-      <c r="E12" t="str">
-        <f>FIXED(orctun_sum_in!H7)</f>
-        <v>0.87</v>
-      </c>
-      <c r="F12" t="str">
-        <f>FIXED(orctun_sum_in!J7)</f>
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="B13" t="str">
-        <f>CONCATENATE("(",FIXED(orctun_sum_in!C7),")")</f>
-        <v>(20.04)</v>
-      </c>
-      <c r="C13" t="str">
-        <f>CONCATENATE("(",FIXED(orctun_sum_in!E7),")")</f>
-        <v>(0.14)</v>
-      </c>
-      <c r="D13" t="str">
-        <f>CONCATENATE("(",FIXED(orctun_sum_in!G7),")")</f>
-        <v>(0.14)</v>
-      </c>
-      <c r="E13" t="str">
-        <f>CONCATENATE("(",FIXED(orctun_sum_in!I7),")")</f>
-        <v>(0.09)</v>
-      </c>
-      <c r="F13" t="str">
-        <f>CONCATENATE("(",FIXED(orctun_sum_in!K7),")")</f>
         <v>(0.22)</v>
       </c>
     </row>
@@ -3807,7 +4700,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A2:A7"/>
@@ -3815,7 +4708,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -3824,37 +4717,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -4030,41 +4923,6 @@
       </c>
       <c r="K6">
         <v>0.22159541323000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>26.747835036400001</v>
-      </c>
-      <c r="C7">
-        <v>20.035565399599999</v>
-      </c>
-      <c r="D7">
-        <v>0.68629856452399995</v>
-      </c>
-      <c r="E7">
-        <v>0.14325939175999999</v>
-      </c>
-      <c r="F7">
-        <v>0.62846590909099997</v>
-      </c>
-      <c r="G7">
-        <v>0.13592395862600001</v>
-      </c>
-      <c r="H7">
-        <v>0.87012237639000001</v>
-      </c>
-      <c r="I7">
-        <v>8.5121457090899993E-2</v>
-      </c>
-      <c r="J7">
-        <v>0.59272693281699995</v>
-      </c>
-      <c r="K7">
-        <v>0.217427239479</v>
       </c>
     </row>
   </sheetData>
@@ -4088,42 +4946,42 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" t="s">
-        <v>99</v>
-      </c>
       <c r="K1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B2, 5))</f>
@@ -4218,7 +5076,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B3, 5))</f>
@@ -4313,7 +5171,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B4, 5))</f>
@@ -4408,7 +5266,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B5, 5))</f>
@@ -4503,7 +5361,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B6, 5))</f>
@@ -4598,7 +5456,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B7, 5))</f>
@@ -4693,7 +5551,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B8, 5))</f>
@@ -4788,7 +5646,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B9, 5))</f>
@@ -4883,7 +5741,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B18" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B10, 5))</f>
@@ -4978,7 +5836,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B20" s="2" t="str">
         <f>FIXED(LEFT(cvmse_sim_in!B11, 5))</f>
@@ -5482,7 +6340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -5490,30 +6348,30 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B2, 5))</f>
@@ -5535,9 +6393,9 @@
         <f>FIXED(LEFT(orctun_sim_in!F2, 5))</f>
         <v>0.86</v>
       </c>
-      <c r="G2" s="2" t="str">
+      <c r="G2" s="2" t="e">
         <f>FIXED(LEFT(orctun_sim_in!G2, 5))</f>
-        <v>0.93</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -5565,9 +6423,9 @@
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!F2,8, 5)),")")</f>
         <v>(0.06)</v>
       </c>
-      <c r="G3" s="1" t="str">
+      <c r="G3" s="1" t="e">
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!G2,8, 5)),")")</f>
-        <v>(0.03)</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -5576,7 +6434,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B3, 5))</f>
@@ -5598,9 +6456,9 @@
         <f>FIXED(LEFT(orctun_sim_in!F3, 5))</f>
         <v>0.93</v>
       </c>
-      <c r="G4" s="2" t="str">
+      <c r="G4" s="2" t="e">
         <f>FIXED(LEFT(orctun_sim_in!G3, 5))</f>
-        <v>0.92</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -5628,9 +6486,9 @@
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!F3,8, 5)),")")</f>
         <v>(0.02)</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="G5" s="1" t="e">
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!G3,8, 5)),")")</f>
-        <v>(0.02)</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -5639,7 +6497,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B4, 5))</f>
@@ -5661,9 +6519,9 @@
         <f>FIXED(LEFT(orctun_sim_in!F4, 5))</f>
         <v>0.92</v>
       </c>
-      <c r="G6" s="2" t="str">
+      <c r="G6" s="2" t="e">
         <f>FIXED(LEFT(orctun_sim_in!G4, 5))</f>
-        <v>0.86</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -5691,9 +6549,9 @@
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!F4,8, 5)),")")</f>
         <v>(0.03)</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="G7" s="1" t="e">
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!G4,8, 5)),")")</f>
-        <v>(0.08)</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -5702,7 +6560,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>FIXED(LEFT(orctun_sim_in!B5, 5))</f>
@@ -5724,9 +6582,9 @@
         <f>FIXED(LEFT(orctun_sim_in!F5, 5))</f>
         <v>0.98</v>
       </c>
-      <c r="G8" s="2" t="str">
+      <c r="G8" s="2" t="e">
         <f>FIXED(LEFT(orctun_sim_in!G5, 5))</f>
-        <v>0.85</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -5754,9 +6612,9 @@
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!F5,8, 5)),")")</f>
         <v>(0.01)</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="G9" s="1" t="e">
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!G5,8, 5)),")")</f>
-        <v>(0.05)</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -5765,31 +6623,31 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!B6, 5))</f>
-        <v>0.86</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!C6, 5))</f>
-        <v>0.93</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!D6, 5))</f>
-        <v>0.92</v>
-      </c>
-      <c r="E10" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!E6, 5))</f>
-        <v>0.98</v>
-      </c>
-      <c r="F10" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!F6, 5))</f>
-        <v>1.00</v>
-      </c>
-      <c r="G10" s="2" t="str">
+        <v>89</v>
+      </c>
+      <c r="B10" s="2" t="e">
+        <f>FIXED(LEFT(orctun_sim_in!#REF!, 5))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C10" s="2" t="e">
+        <f>FIXED(LEFT(orctun_sim_in!#REF!, 5))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D10" s="2" t="e">
+        <f>FIXED(LEFT(orctun_sim_in!#REF!, 5))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E10" s="2" t="e">
+        <f>FIXED(LEFT(orctun_sim_in!#REF!, 5))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F10" s="2" t="e">
+        <f>FIXED(LEFT(orctun_sim_in!#REF!, 5))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G10" s="2" t="e">
         <f>FIXED(LEFT(orctun_sim_in!G6, 5))</f>
-        <v>0.86</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -5797,29 +6655,29 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="B11" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!B6,8, 5)),")")</f>
-        <v>(0.06)</v>
-      </c>
-      <c r="C11" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!C6,8, 5)),")")</f>
-        <v>(0.02)</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!D6,8, 5)),")")</f>
-        <v>(0.03)</v>
-      </c>
-      <c r="E11" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!E6,8, 5)),")")</f>
-        <v>(0.01)</v>
-      </c>
-      <c r="F11" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!F6,8, 5)),")")</f>
-        <v>(0.00)</v>
-      </c>
-      <c r="G11" s="1" t="str">
+      <c r="B11" s="1" t="e">
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!#REF!,8, 5)),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C11" s="1" t="e">
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!#REF!,8, 5)),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D11" s="1" t="e">
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!#REF!,8, 5)),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E11" s="1" t="e">
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!#REF!,8, 5)),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F11" s="1" t="e">
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!#REF!,8, 5)),")")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G11" s="1" t="e">
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!G6,8, 5)),")")</f>
-        <v>(0.04)</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -5828,31 +6686,31 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!B7, 5))</f>
+        <f>FIXED(LEFT(orctun_sim_in!B6, 5))</f>
+        <v>0.86</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f>FIXED(LEFT(orctun_sim_in!C6, 5))</f>
         <v>0.93</v>
       </c>
-      <c r="C12" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!C7, 5))</f>
+      <c r="D12" s="2" t="str">
+        <f>FIXED(LEFT(orctun_sim_in!D6, 5))</f>
         <v>0.92</v>
       </c>
-      <c r="D12" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!D7, 5))</f>
-        <v>0.86</v>
-      </c>
       <c r="E12" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!E7, 5))</f>
-        <v>0.85</v>
+        <f>FIXED(LEFT(orctun_sim_in!E6, 5))</f>
+        <v>0.98</v>
       </c>
       <c r="F12" s="2" t="str">
-        <f>FIXED(LEFT(orctun_sim_in!F7, 5))</f>
-        <v>0.86</v>
-      </c>
-      <c r="G12" s="2" t="str">
+        <f>FIXED(LEFT(orctun_sim_in!F6, 5))</f>
+        <v>1.00</v>
+      </c>
+      <c r="G12" s="2" t="e">
         <f>FIXED(LEFT(orctun_sim_in!G7, 5))</f>
-        <v>1.00</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -5861,28 +6719,28 @@
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!B7,8, 5)),")")</f>
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!B6,8, 5)),")")</f>
+        <v>(0.06)</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!C6,8, 5)),")")</f>
+        <v>(0.02)</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!D6,8, 5)),")")</f>
         <v>(0.03)</v>
       </c>
-      <c r="C13" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!C7,8, 5)),")")</f>
-        <v>(0.02)</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!D7,8, 5)),")")</f>
-        <v>(0.08)</v>
-      </c>
       <c r="E13" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!E7,8, 5)),")")</f>
-        <v>(0.05)</v>
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!E6,8, 5)),")")</f>
+        <v>(0.01)</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!F7,8, 5)),")")</f>
-        <v>(0.04)</v>
-      </c>
-      <c r="G13" s="1" t="str">
+        <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!F6,8, 5)),")")</f>
+        <v>(0.00)</v>
+      </c>
+      <c r="G13" s="1" t="e">
         <f>CONCATENATE("(",FIXED(MID(orctun_sim_in!G7,8, 5)),")")</f>
-        <v>(0.00)</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>

</xml_diff>